<commit_message>
Added TestDataReader Added e2e test
</commit_message>
<xml_diff>
--- a/codeless_test/src/test/resources/suites/test_google.xlsx
+++ b/codeless_test/src/test/resources/suites/test_google.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO5\codeless_ard_1\codeless_test\src\test\resources\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO8\codeless_mastertestdata\codeless_test\src\test\resources\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,10 +14,8 @@
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
     <sheet name="t-googletest" sheetId="9" r:id="rId2"/>
-    <sheet name="d-dataSheet" sheetId="10" r:id="rId3"/>
-    <sheet name="d-dev" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>key</t>
   </si>
@@ -185,102 +183,36 @@
     <t>customer.api.v1.employee.{id}</t>
   </si>
   <si>
-    <t>website</t>
-  </si>
-  <si>
-    <t>dummy.restapiexample.com</t>
-  </si>
-  <si>
-    <t>apiHost</t>
-  </si>
-  <si>
     <t>goto</t>
   </si>
   <si>
-    <t>/api/v1/create</t>
-  </si>
-  <si>
-    <t>apiPath</t>
-  </si>
-  <si>
-    <t>searchElement</t>
-  </si>
-  <si>
     <t>close browser</t>
   </si>
   <si>
     <t>close</t>
   </si>
   <si>
-    <t>https://www.bing.com/</t>
-  </si>
-  <si>
-    <t>searchBar</t>
-  </si>
-  <si>
     <t>Google.googlepage.searchbutton</t>
   </si>
   <si>
-    <t>bing.yahoopage.searchbar</t>
-  </si>
-  <si>
-    <t>bing.yahoopage.searchbutton</t>
-  </si>
-  <si>
-    <t>omdbhost</t>
-  </si>
-  <si>
-    <t>http://www.omdbapi.com</t>
-  </si>
-  <si>
-    <t>omdbpath</t>
-  </si>
-  <si>
-    <t>imdb</t>
-  </si>
-  <si>
-    <t>?apikey=91999f16&amp;i=tt0910970</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
     <t>customer.api.v1.delete.{id}</t>
   </si>
   <si>
-    <t>https://www.imdb.com/title/tt1049413/</t>
-  </si>
-  <si>
-    <t>https://www.imdb.com/title/tt0910970/</t>
-  </si>
-  <si>
-    <t>imdb2</t>
-  </si>
-  <si>
     <t>waitTime::6000</t>
   </si>
   <si>
-    <t>https://www.imdb.com</t>
-  </si>
-  <si>
-    <t>imdbhome</t>
-  </si>
-  <si>
     <t>waitType::clickable</t>
   </si>
   <si>
     <t>Navigate to UI page</t>
   </si>
   <si>
-    <t>search</t>
-  </si>
-  <si>
     <t>click search button</t>
   </si>
   <si>
-    <t>t-mobile best network</t>
-  </si>
-  <si>
     <t>path::id::{{empId}}</t>
   </si>
   <si>
@@ -312,6 +244,9 @@
   </si>
   <si>
     <t>webdriver.tunnelIdentifier</t>
+  </si>
+  <si>
+    <t>testdata.filename</t>
   </si>
 </sst>
 </file>
@@ -404,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -433,7 +368,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -715,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -891,13 +825,13 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B17" s="15"/>
     </row>
@@ -907,6 +841,11 @@
       </c>
       <c r="B18" s="11" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -973,7 +912,7 @@
     </row>
     <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
@@ -985,18 +924,18 @@
         <v>50</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
@@ -1008,36 +947,36 @@
         <v>25</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="13" t="s">
@@ -1048,7 +987,7 @@
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>29</v>
@@ -1057,7 +996,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="4"/>
@@ -1065,28 +1004,28 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="13" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1096,179 +1035,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
remove duplicated plugins and update browser capabilities
</commit_message>
<xml_diff>
--- a/codeless_test/src/test/resources/suites/test_google.xlsx
+++ b/codeless_test/src/test/resources/suites/test_google.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skorpu\Documents\feature\SprintTMO8\codeless_mastertestdata\codeless_test\src\test\resources\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jung\Documents\codeless\codeless_test\src\test\resources\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE6723C-00CA-4C02-8CC9-ACC40CF22F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13176" windowHeight="6408" activeTab="1"/>
+    <workbookView xWindow="3630" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -78,181 +79,181 @@
     <t>web_drivers/windows/chromedriver.exe</t>
   </si>
   <si>
+    <t>serviceCall</t>
+  </si>
+  <si>
+    <t>webdriver.path.firefox</t>
+  </si>
+  <si>
+    <t>web_drivers/windows/geckodriver.exe</t>
+  </si>
+  <si>
+    <t>Path to the firefox webdriver to use for this machine. Installed under &lt;INSTALL_DIR&gt;/webdrivers/&lt;OS&gt; by default. For Windows: web_drivers/windows/geckodriver.exe For Mac: web_drivers/mac/geckodriver</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>Google.googlepage.searchbar</t>
+  </si>
+  <si>
+    <t>https://www.google.com/</t>
+  </si>
+  <si>
+    <t>sendKeys</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Plateform type for remote web driver intializing</t>
+  </si>
+  <si>
+    <t>Version for plateform type selected</t>
+  </si>
+  <si>
+    <t>macos 10.12</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>webdriver.hub</t>
+  </si>
+  <si>
+    <t>logging.details.enabled</t>
+  </si>
+  <si>
+    <t>customer.api.v1.create</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>customer.api.v1.employee.{id}</t>
+  </si>
+  <si>
+    <t>goto</t>
+  </si>
+  <si>
+    <t>close browser</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>Google.googlepage.searchbutton</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>customer.api.v1.delete.{id}</t>
+  </si>
+  <si>
+    <t>waitTime::6000</t>
+  </si>
+  <si>
+    <t>waitType::clickable</t>
+  </si>
+  <si>
+    <t>Navigate to UI page</t>
+  </si>
+  <si>
+    <t>click search button</t>
+  </si>
+  <si>
+    <t>path::id::{{empId}}</t>
+  </si>
+  <si>
+    <t>export::empId::JSONPATH::id</t>
+  </si>
+  <si>
+    <t>export::empsalary::JSONPATH::salary</t>
+  </si>
+  <si>
+    <t>{{empsalary}}</t>
+  </si>
+  <si>
+    <t>GET call from customer api</t>
+  </si>
+  <si>
+    <t>POST call to customer api</t>
+  </si>
+  <si>
+    <t>type salary of employee created</t>
+  </si>
+  <si>
+    <t>body::string::{"name":"etptest","salary":"123456789","age":"100"}</t>
+  </si>
+  <si>
+    <t>delete call from customer api</t>
+  </si>
+  <si>
+    <t>webdriver.parentTunnel</t>
+  </si>
+  <si>
+    <t>webdriver.tunnelIdentifier</t>
+  </si>
+  <si>
+    <t>testdata.filename</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.chrome</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.chrome</t>
+  </si>
+  <si>
+    <t>91.0</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.firefox</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.safari</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.firefox</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.safari</t>
+  </si>
+  <si>
+    <t>webdriver.platformName.edge</t>
+  </si>
+  <si>
+    <t>webdriver.browserVersion.edge</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>webdriver.path.edge</t>
+  </si>
+  <si>
+    <t>web_drivers/windows/msedgedriver.exe</t>
+  </si>
+  <si>
+    <t>Path to the edge webdriver to use for this machine. Installed under &lt;INSTALL_DIR&gt;/webdrivers/&lt;OS&gt; by default. Windows only, no other valid settings.</t>
+  </si>
+  <si>
     <t>chrome</t>
-  </si>
-  <si>
-    <t>serviceCall</t>
-  </si>
-  <si>
-    <t>webdriver.path.firefox</t>
-  </si>
-  <si>
-    <t>web_drivers/windows/geckodriver.exe</t>
-  </si>
-  <si>
-    <t>Path to the firefox webdriver to use for this machine. Installed under &lt;INSTALL_DIR&gt;/webdrivers/&lt;OS&gt; by default. For Windows: web_drivers/windows/geckodriver.exe For Mac: web_drivers/mac/geckodriver</t>
-  </si>
-  <si>
-    <t>webdriver.path.ie</t>
-  </si>
-  <si>
-    <t>web_drivers/windows/IEDriverServer.exe</t>
-  </si>
-  <si>
-    <t>Path to the ie webdriver to use for this machine. Installed under &lt;INSTALL_DIR&gt;/webdrivers/&lt;OS&gt; by default. Windows only, no other valid settings.</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>Google.googlepage.searchbar</t>
-  </si>
-  <si>
-    <t>https://www.google.com/</t>
-  </si>
-  <si>
-    <t>sendKeys</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>webdriver.platform.chrome</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
-    <t>Plateform type for remote web driver intializing</t>
-  </si>
-  <si>
-    <t>webdriver.version.chrome</t>
-  </si>
-  <si>
-    <t>61.0</t>
-  </si>
-  <si>
-    <t>Version for plateform type selected</t>
-  </si>
-  <si>
-    <t>webdriver.platform.ie</t>
-  </si>
-  <si>
-    <t>webdriver.version.ie</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>webdriver.platform.firefox</t>
-  </si>
-  <si>
-    <t>webdriver.version.firefox</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>webdriver.platform.safari</t>
-  </si>
-  <si>
-    <t>macos 10.12</t>
-  </si>
-  <si>
-    <t>webdriver.version.safari</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>webdriver.hub</t>
-  </si>
-  <si>
-    <t>logging.details.enabled</t>
-  </si>
-  <si>
-    <t>customer.api.v1.create</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>customer.api.v1.employee.{id}</t>
-  </si>
-  <si>
-    <t>goto</t>
-  </si>
-  <si>
-    <t>close browser</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>Google.googlepage.searchbutton</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>customer.api.v1.delete.{id}</t>
-  </si>
-  <si>
-    <t>waitTime::6000</t>
-  </si>
-  <si>
-    <t>waitType::clickable</t>
-  </si>
-  <si>
-    <t>Navigate to UI page</t>
-  </si>
-  <si>
-    <t>click search button</t>
-  </si>
-  <si>
-    <t>path::id::{{empId}}</t>
-  </si>
-  <si>
-    <t>export::empId::JSONPATH::id</t>
-  </si>
-  <si>
-    <t>export::empsalary::JSONPATH::salary</t>
-  </si>
-  <si>
-    <t>{{empsalary}}</t>
-  </si>
-  <si>
-    <t>GET call from customer api</t>
-  </si>
-  <si>
-    <t>POST call to customer api</t>
-  </si>
-  <si>
-    <t>type salary of employee created</t>
-  </si>
-  <si>
-    <t>body::string::{"name":"etptest","salary":"123456789","age":"100"}</t>
-  </si>
-  <si>
-    <t>delete call from customer api</t>
-  </si>
-  <si>
-    <t>webdriver.parentTunnel</t>
-  </si>
-  <si>
-    <t>webdriver.tunnelIdentifier</t>
-  </si>
-  <si>
-    <t>testdata.filename</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,22 +649,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="7"/>
+    <col min="3" max="3" width="62.42578125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -674,29 +675,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -707,145 +708,145 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -855,27 +856,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -899,7 +900,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -910,125 +911,125 @@
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" s="13"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="13" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
     </row>
   </sheetData>

</xml_diff>